<commit_message>
First Demo for excel
</commit_message>
<xml_diff>
--- a/Email/output.xlsx
+++ b/Email/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,30 +444,75 @@
           <t>summary</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>venue</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>7th Dec 2023, 10am</t>
+          <t>2023-11-29 14:45:20+08:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AI Research Seminar (AIRS) Series</t>
+          <t>Student - Lim Qin Xin - Startup Springboard</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Microsoft Teams Meeting</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>8th Dec 2023, 12pm</t>
+          <t>2023-11-29 14:39:47+08:00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Good food!</t>
-        </is>
-      </c>
+          <t>Week 12 Cohort 2 In-class Annotation</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-11-29 14:23:00+08:00</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>arrangement for MA in Week 13 and 14</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-11-29 11:48:36+08:00</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Something's Brewing! Accenture University Innovation Challenge 2024</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>